<commit_message>
Refactor : ItemManager 주석 추가
</commit_message>
<xml_diff>
--- a/Assets/Excel/Items/ConsumableDB_Sheet.xlsx
+++ b/Assets/Excel/Items/ConsumableDB_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\babyg\Desktop\Coding\unity\Sisyphus\Assets\Excel\Items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9592F25-300E-40B4-8ED1-E35E7A4BF92F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2A3726-B5E4-45AD-A135-393CB58AE068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="1050" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -443,7 +443,7 @@
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -606,10 +606,10 @@
         <v>0</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O3">
         <v>0</v>

</xml_diff>